<commit_message>
adding a picture of choice
</commit_message>
<xml_diff>
--- a/images.xlsx
+++ b/images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shach\3rd_year_ex\final_project\project03.5\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F45CA2-CFF3-4984-BB59-4E60B9424057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498CC7CF-9ED6-4551-A52C-94932511398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -27,510 +27,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="173">
   <si>
-    <t>'fn_450_12_900.ppm'</t>
-  </si>
-  <si>
     <t>'People'</t>
   </si>
   <si>
     <t>'225.00'</t>
   </si>
   <si>
-    <t>'fn_450_31_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_13_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_19_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_2_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_20_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_23_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_39_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_40_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_10_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_38_900.ppm'</t>
-  </si>
-  <si>
     <t>'Face'</t>
   </si>
   <si>
-    <t>'fn_450_24_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_5_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_25_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_8_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_4_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_22_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_27_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_30_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_21_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_34_900.ppm'</t>
-  </si>
-  <si>
     <t>'Indoor'</t>
   </si>
   <si>
-    <t>'fn_450_17_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_35_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_33_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_15_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_36_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_37_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_7_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_32_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_14_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_9_900.ppm'</t>
-  </si>
-  <si>
     <t>'Outdoor'</t>
   </si>
   <si>
-    <t>'fn_450_29_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_3_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_18_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_26_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_28_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_16_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_11_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_1_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_450_6_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_24_900.ppm'</t>
-  </si>
-  <si>
     <t>'450.00'</t>
   </si>
   <si>
-    <t>'fn_225_17_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_5_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_22_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_19_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_10_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_3_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_7_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_36_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_25_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_2_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_29_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_4_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_11_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_26_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_9_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_40_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_16_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_30_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_15_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_37_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_33_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_28_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_32_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_39_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_38_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_23_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_20_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_35_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_21_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_1_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_18_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_14_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_27_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_34_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_31_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_12_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_13_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_8_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_225_6_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_13_900.ppm'</t>
-  </si>
-  <si>
     <t>'900.00'</t>
   </si>
   <si>
-    <t>'fn_112_12_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_21_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_24_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_1_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_33_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_17_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_16_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_32_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_26_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_40_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_38_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_30_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_22_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_28_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_8_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_25_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_31_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_37_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_39_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_34_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_20_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_36_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_18_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_14_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_29_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_15_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_23_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_35_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_27_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_3_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_2_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_7_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_19_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_10_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_9_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_4_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_11_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_5_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_112_6_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_8_900.ppm'</t>
-  </si>
-  <si>
     <t>'112.00'</t>
   </si>
   <si>
-    <t>'fn_900_16_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_38_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_4_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_17_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_1_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_14_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_24_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_3_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_15_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_2_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_25_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_36_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_6_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_40_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_27_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_35_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_39_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_28_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_37_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_30_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_26_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_32_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_23_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_22_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_34_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_31_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_21_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_29_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_33_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_10_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_9_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_12_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_5_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_7_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_20_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_13_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_18_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_19_900.ppm'</t>
-  </si>
-  <si>
-    <t>'fn_900_11_900.ppm'</t>
-  </si>
-  <si>
     <t>image_name</t>
   </si>
   <si>
@@ -544,6 +64,486 @@
   </si>
   <si>
     <t>image_size</t>
+  </si>
+  <si>
+    <t>fn_450_31_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_13_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_19_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_2_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_20_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_23_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_39_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_40_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_10_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_38_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_24_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_5_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_25_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_8_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_4_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_22_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_27_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_30_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_21_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_34_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_17_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_35_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_33_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_15_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_36_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_37_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_7_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_32_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_14_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_9_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_29_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_3_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_18_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_26_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_28_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_16_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_11_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_1_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_6_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_24_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_17_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_5_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_22_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_19_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_10_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_3_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_7_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_36_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_25_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_2_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_29_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_4_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_11_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_26_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_9_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_40_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_16_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_30_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_15_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_37_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_33_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_28_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_32_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_39_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_38_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_23_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_20_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_35_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_21_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_1_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_18_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_14_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_27_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_34_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_31_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_12_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_13_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_8_900.png'</t>
+  </si>
+  <si>
+    <t>fn_225_6_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_13_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_12_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_21_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_24_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_1_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_33_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_17_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_16_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_32_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_26_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_40_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_38_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_30_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_22_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_28_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_8_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_25_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_31_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_37_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_39_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_34_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_20_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_36_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_18_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_14_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_29_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_15_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_23_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_35_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_27_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_3_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_2_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_7_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_19_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_10_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_9_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_4_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_11_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_5_900.png'</t>
+  </si>
+  <si>
+    <t>fn_112_6_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_8_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_16_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_38_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_4_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_17_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_1_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_14_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_24_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_3_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_15_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_2_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_25_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_36_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_6_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_40_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_27_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_35_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_39_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_28_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_37_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_30_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_26_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_32_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_23_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_22_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_34_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_31_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_21_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_29_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_33_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_10_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_9_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_12_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_5_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_7_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_20_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_13_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_18_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_19_900.png'</t>
+  </si>
+  <si>
+    <t>fn_900_11_900.png'</t>
+  </si>
+  <si>
+    <t>fn_450_12_900.png'</t>
   </si>
 </sst>
 </file>
@@ -579,8 +579,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,37 +865,40 @@
   <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>83</v>
@@ -904,14 +908,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>104</v>
@@ -921,14 +925,14 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>84</v>
@@ -938,14 +942,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>90</v>
@@ -955,14 +959,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>102</v>
@@ -972,14 +976,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="A7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>92</v>
@@ -989,14 +993,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
+      <c r="A8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>95</v>
@@ -1006,14 +1010,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="A9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>112</v>
@@ -1023,14 +1027,14 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>114</v>
@@ -1040,14 +1044,14 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
+      <c r="A11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>81</v>
@@ -1057,14 +1061,14 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
+      <c r="A12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>111</v>
@@ -1074,14 +1078,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
+      <c r="A13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>96</v>
@@ -1091,14 +1095,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
+      <c r="A14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>116</v>
@@ -1108,14 +1112,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
+      <c r="A15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>97</v>
@@ -1125,14 +1129,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
+      <c r="A16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>119</v>
@@ -1142,14 +1146,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
+      <c r="A17" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>115</v>
@@ -1159,14 +1163,14 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>94</v>
@@ -1176,14 +1180,14 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
+      <c r="A19" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>99</v>
@@ -1193,14 +1197,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
+      <c r="A20" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>103</v>
@@ -1210,14 +1214,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
+      <c r="A21" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>93</v>
@@ -1227,14 +1231,14 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
+      <c r="A22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>107</v>
@@ -1244,14 +1248,14 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
+      <c r="A23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>88</v>
@@ -1261,14 +1265,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
+      <c r="A24" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>108</v>
@@ -1278,14 +1282,14 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>27</v>
+      <c r="A25" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>106</v>
@@ -1295,14 +1299,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
+      <c r="A26" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>86</v>
@@ -1312,14 +1316,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
+      <c r="A27" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>109</v>
@@ -1329,14 +1333,14 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
+      <c r="A28" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>110</v>
@@ -1346,14 +1350,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>31</v>
+      <c r="A29" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>118</v>
@@ -1363,14 +1367,14 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
+      <c r="A30" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>105</v>
@@ -1380,14 +1384,14 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>33</v>
+      <c r="A31" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>85</v>
@@ -1397,14 +1401,14 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>34</v>
+      <c r="A32" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>120</v>
@@ -1414,14 +1418,14 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>36</v>
+      <c r="A33" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>101</v>
@@ -1431,14 +1435,14 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>37</v>
+      <c r="A34" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>113</v>
@@ -1448,14 +1452,14 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>38</v>
+      <c r="A35" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>89</v>
@@ -1465,14 +1469,14 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>39</v>
+      <c r="A36" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>98</v>
@@ -1482,14 +1486,14 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>40</v>
+      <c r="A37" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>100</v>
@@ -1499,14 +1503,14 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>41</v>
+      <c r="A38" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>87</v>
@@ -1516,14 +1520,14 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>42</v>
+      <c r="A39" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>82</v>
@@ -1533,14 +1537,14 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>43</v>
+      <c r="A40" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>91</v>
@@ -1550,14 +1554,14 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>44</v>
+      <c r="A41" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>117</v>
@@ -1567,14 +1571,14 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>45</v>
+      <c r="A42" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>56</v>
@@ -1584,14 +1588,14 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>47</v>
+      <c r="A43" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>48</v>
@@ -1601,14 +1605,14 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>48</v>
+      <c r="A44" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>76</v>
@@ -1618,14 +1622,14 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>49</v>
+      <c r="A45" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>54</v>
@@ -1635,14 +1639,14 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>50</v>
+      <c r="A46" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>50</v>
@@ -1652,14 +1656,14 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>51</v>
+      <c r="A47" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>41</v>
@@ -1669,14 +1673,14 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>52</v>
+      <c r="A48" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>73</v>
@@ -1686,14 +1690,14 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>53</v>
+      <c r="A49" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>78</v>
@@ -1703,14 +1707,14 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>54</v>
+      <c r="A50" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>69</v>
@@ -1720,14 +1724,14 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>55</v>
+      <c r="A51" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D51">
         <v>57</v>
@@ -1737,14 +1741,14 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>56</v>
+      <c r="A52" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>62</v>
@@ -1754,14 +1758,14 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>57</v>
+      <c r="A53" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>61</v>
@@ -1771,14 +1775,14 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>58</v>
+      <c r="A54" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D54">
         <v>75</v>
@@ -1788,14 +1792,14 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>59</v>
+      <c r="A55" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>42</v>
@@ -1805,14 +1809,14 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>60</v>
+      <c r="A56" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>58</v>
@@ -1822,14 +1826,14 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>61</v>
+      <c r="A57" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D57">
         <v>80</v>
@@ -1839,14 +1843,14 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>62</v>
+      <c r="A58" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D58">
         <v>74</v>
@@ -1856,14 +1860,14 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>63</v>
+      <c r="A59" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D59">
         <v>47</v>
@@ -1873,14 +1877,14 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>64</v>
+      <c r="A60" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D60">
         <v>63</v>
@@ -1890,14 +1894,14 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>65</v>
+      <c r="A61" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <v>46</v>
@@ -1907,14 +1911,14 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>66</v>
+      <c r="A62" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D62">
         <v>70</v>
@@ -1924,14 +1928,14 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>67</v>
+      <c r="A63" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D63">
         <v>66</v>
@@ -1941,14 +1945,14 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>68</v>
+      <c r="A64" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D64">
         <v>60</v>
@@ -1958,14 +1962,14 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>69</v>
+      <c r="A65" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>65</v>
@@ -1975,14 +1979,14 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>70</v>
+      <c r="A66" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D66">
         <v>72</v>
@@ -1992,14 +1996,14 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>71</v>
+      <c r="A67" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D67">
         <v>71</v>
@@ -2009,14 +2013,14 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>72</v>
+      <c r="A68" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D68">
         <v>55</v>
@@ -2026,14 +2030,14 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>73</v>
+      <c r="A69" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <v>52</v>
@@ -2043,14 +2047,14 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>74</v>
+      <c r="A70" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>68</v>
@@ -2060,14 +2064,14 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>75</v>
+      <c r="A71" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D71">
         <v>53</v>
@@ -2077,14 +2081,14 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>76</v>
+      <c r="A72" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D72">
         <v>51</v>
@@ -2094,14 +2098,14 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>77</v>
+      <c r="A73" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D73">
         <v>49</v>
@@ -2111,14 +2115,14 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>78</v>
+      <c r="A74" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D74">
         <v>45</v>
@@ -2128,14 +2132,14 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>79</v>
+      <c r="A75" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D75">
         <v>59</v>
@@ -2145,14 +2149,14 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>80</v>
+      <c r="A76" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D76">
         <v>67</v>
@@ -2162,14 +2166,14 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>81</v>
+      <c r="A77" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D77">
         <v>64</v>
@@ -2179,14 +2183,14 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>82</v>
+      <c r="A78" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D78">
         <v>43</v>
@@ -2196,14 +2200,14 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>83</v>
+      <c r="A79" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D79">
         <v>44</v>
@@ -2213,14 +2217,14 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>84</v>
+      <c r="A80" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D80">
         <v>79</v>
@@ -2230,14 +2234,14 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>85</v>
+      <c r="A81" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D81">
         <v>77</v>
@@ -2247,14 +2251,14 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>86</v>
+      <c r="A82" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D82">
         <v>4</v>
@@ -2264,14 +2268,14 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>88</v>
+      <c r="A83" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D83">
         <v>3</v>
@@ -2281,14 +2285,14 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>89</v>
+      <c r="A84" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D84">
         <v>13</v>
@@ -2298,14 +2302,14 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>90</v>
+      <c r="A85" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D85">
         <v>16</v>
@@ -2315,14 +2319,14 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>91</v>
+      <c r="A86" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D86">
         <v>11</v>
@@ -2332,14 +2336,14 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>92</v>
+      <c r="A87" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D87">
         <v>26</v>
@@ -2349,14 +2353,14 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>93</v>
+      <c r="A88" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D88">
         <v>8</v>
@@ -2366,14 +2370,14 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>94</v>
+      <c r="A89" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D89">
         <v>7</v>
@@ -2383,14 +2387,14 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>95</v>
+      <c r="A90" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="B90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D90">
         <v>25</v>
@@ -2400,14 +2404,14 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>96</v>
+      <c r="A91" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D91">
         <v>18</v>
@@ -2417,14 +2421,14 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>97</v>
+      <c r="A92" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D92">
         <v>34</v>
@@ -2434,14 +2438,14 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>98</v>
+      <c r="A93" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D93">
         <v>31</v>
@@ -2451,14 +2455,14 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>99</v>
+      <c r="A94" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D94">
         <v>23</v>
@@ -2468,14 +2472,14 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>100</v>
+      <c r="A95" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D95">
         <v>14</v>
@@ -2485,14 +2489,14 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>101</v>
+      <c r="A96" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B96" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D96">
         <v>20</v>
@@ -2502,14 +2506,14 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>102</v>
+      <c r="A97" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D97">
         <v>39</v>
@@ -2519,14 +2523,14 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>103</v>
+      <c r="A98" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D98">
         <v>17</v>
@@ -2536,14 +2540,14 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>104</v>
+      <c r="A99" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D99">
         <v>24</v>
@@ -2553,14 +2557,14 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>105</v>
+      <c r="A100" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D100">
         <v>30</v>
@@ -2570,14 +2574,14 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>106</v>
+      <c r="A101" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D101">
         <v>32</v>
@@ -2587,14 +2591,14 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>107</v>
+      <c r="A102" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D102">
         <v>27</v>
@@ -2604,14 +2608,14 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>108</v>
+      <c r="A103" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D103">
         <v>12</v>
@@ -2621,14 +2625,14 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>109</v>
+      <c r="A104" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D104">
         <v>29</v>
@@ -2638,14 +2642,14 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>110</v>
+      <c r="A105" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D105">
         <v>9</v>
@@ -2655,14 +2659,14 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>111</v>
+      <c r="A106" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D106">
         <v>5</v>
@@ -2672,14 +2676,14 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>112</v>
+      <c r="A107" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D107">
         <v>21</v>
@@ -2689,14 +2693,14 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>113</v>
+      <c r="A108" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D108">
         <v>6</v>
@@ -2706,14 +2710,14 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>114</v>
+      <c r="A109" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D109">
         <v>15</v>
@@ -2723,14 +2727,14 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>115</v>
+      <c r="A110" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B110" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D110">
         <v>28</v>
@@ -2740,14 +2744,14 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>116</v>
+      <c r="A111" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B111" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D111">
         <v>19</v>
@@ -2757,14 +2761,14 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>117</v>
+      <c r="A112" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D112">
         <v>33</v>
@@ -2774,14 +2778,14 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>118</v>
+      <c r="A113" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C113" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D113">
         <v>22</v>
@@ -2791,14 +2795,14 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>119</v>
+      <c r="A114" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D114">
         <v>38</v>
@@ -2808,14 +2812,14 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>120</v>
+      <c r="A115" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="B115" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D115">
         <v>10</v>
@@ -2825,14 +2829,14 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>121</v>
+      <c r="A116" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -2842,14 +2846,14 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>122</v>
+      <c r="A117" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B117" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D117">
         <v>40</v>
@@ -2859,14 +2863,14 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>123</v>
+      <c r="A118" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B118" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D118">
         <v>35</v>
@@ -2876,14 +2880,14 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>124</v>
+      <c r="A119" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D119">
         <v>2</v>
@@ -2893,14 +2897,14 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>125</v>
+      <c r="A120" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B120" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D120">
         <v>36</v>
@@ -2910,14 +2914,14 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>126</v>
+      <c r="A121" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="B121" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D121">
         <v>37</v>
@@ -2927,14 +2931,14 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>127</v>
+      <c r="A122" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D122">
         <v>159</v>
@@ -2944,14 +2948,14 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>129</v>
+      <c r="A123" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B123" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D123">
         <v>127</v>
@@ -2961,14 +2965,14 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>130</v>
+      <c r="A124" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="B124" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D124">
         <v>151</v>
@@ -2978,14 +2982,14 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>131</v>
+      <c r="A125" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B125" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D125">
         <v>155</v>
@@ -2995,14 +2999,14 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>132</v>
+      <c r="A126" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B126" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D126">
         <v>128</v>
@@ -3012,14 +3016,14 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>133</v>
+      <c r="A127" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="B127" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D127">
         <v>131</v>
@@ -3029,14 +3033,14 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>134</v>
+      <c r="A128" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="B128" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C128" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D128">
         <v>125</v>
@@ -3046,14 +3050,14 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>135</v>
+      <c r="A129" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="B129" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D129">
         <v>136</v>
@@ -3063,14 +3067,14 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>136</v>
+      <c r="A130" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C130" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D130">
         <v>153</v>
@@ -3080,14 +3084,14 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>137</v>
+      <c r="A131" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="B131" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D131">
         <v>126</v>
@@ -3097,14 +3101,14 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>138</v>
+      <c r="A132" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="B132" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C132" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D132">
         <v>142</v>
@@ -3114,14 +3118,14 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>139</v>
+      <c r="A133" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D133">
         <v>137</v>
@@ -3131,14 +3135,14 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>140</v>
+      <c r="A134" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D134">
         <v>149</v>
@@ -3148,14 +3152,14 @@
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>141</v>
+      <c r="A135" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C135" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D135">
         <v>157</v>
@@ -3165,14 +3169,14 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>142</v>
+      <c r="A136" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C136" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D136">
         <v>154</v>
@@ -3182,14 +3186,14 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>143</v>
+      <c r="A137" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C137" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D137">
         <v>139</v>
@@ -3199,14 +3203,14 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>144</v>
+      <c r="A138" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D138">
         <v>148</v>
@@ -3216,14 +3220,14 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>145</v>
+      <c r="A139" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D139">
         <v>152</v>
@@ -3233,14 +3237,14 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>146</v>
+      <c r="A140" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B140" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D140">
         <v>140</v>
@@ -3250,14 +3254,14 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>147</v>
+      <c r="A141" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="B141" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D141">
         <v>150</v>
@@ -3267,14 +3271,14 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>148</v>
+      <c r="A142" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B142" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D142">
         <v>143</v>
@@ -3284,14 +3288,14 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>149</v>
+      <c r="A143" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B143" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D143">
         <v>138</v>
@@ -3301,14 +3305,14 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>150</v>
+      <c r="A144" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B144" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D144">
         <v>145</v>
@@ -3318,14 +3322,14 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>151</v>
+      <c r="A145" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D145">
         <v>135</v>
@@ -3335,14 +3339,14 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>152</v>
+      <c r="A146" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C146" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D146">
         <v>134</v>
@@ -3352,14 +3356,14 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>153</v>
+      <c r="A147" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="B147" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C147" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D147">
         <v>147</v>
@@ -3369,14 +3373,14 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>154</v>
+      <c r="A148" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="B148" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C148" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D148">
         <v>144</v>
@@ -3386,14 +3390,14 @@
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>155</v>
+      <c r="A149" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B149" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C149" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D149">
         <v>133</v>
@@ -3403,14 +3407,14 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>156</v>
+      <c r="A150" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C150" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D150">
         <v>141</v>
@@ -3420,14 +3424,14 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>157</v>
+      <c r="A151" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B151" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C151" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D151">
         <v>146</v>
@@ -3437,14 +3441,14 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>158</v>
+      <c r="A152" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="B152" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D152">
         <v>121</v>
@@ -3454,14 +3458,14 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>159</v>
+      <c r="A153" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="B153" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D153">
         <v>160</v>
@@ -3471,14 +3475,14 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>160</v>
+      <c r="A154" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B154" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C154" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D154">
         <v>123</v>
@@ -3488,14 +3492,14 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>161</v>
+      <c r="A155" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="B155" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D155">
         <v>156</v>
@@ -3505,14 +3509,14 @@
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>162</v>
+      <c r="A156" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="B156" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D156">
         <v>158</v>
@@ -3522,14 +3526,14 @@
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>163</v>
+      <c r="A157" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="B157" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D157">
         <v>132</v>
@@ -3539,14 +3543,14 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>164</v>
+      <c r="A158" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="B158" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D158">
         <v>124</v>
@@ -3556,14 +3560,14 @@
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>165</v>
+      <c r="A159" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="B159" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C159" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D159">
         <v>129</v>
@@ -3573,14 +3577,14 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>166</v>
+      <c r="A160" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="B160" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D160">
         <v>130</v>
@@ -3590,14 +3594,14 @@
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>167</v>
+      <c r="A161" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B161" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C161" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D161">
         <v>122</v>
@@ -3608,5 +3612,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
manually merge of version
</commit_message>
<xml_diff>
--- a/images.xlsx
+++ b/images.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shach\3rd_year_ex\final_project\project03.5\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498CC7CF-9ED6-4551-A52C-94932511398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479F0631-2A26-4841-B09F-7005A46D1CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">גיליון1!$A$1:$E$161</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="174">
   <si>
     <t>'People'</t>
   </si>
@@ -544,6 +547,9 @@
   </si>
   <si>
     <t>fn_450_12_900.png'</t>
+  </si>
+  <si>
+    <t>miss</t>
   </si>
 </sst>
 </file>
@@ -559,12 +565,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -579,9 +609,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,15 +898,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E161"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,7 +930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -907,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -924,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -941,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -958,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -975,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -992,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1009,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1026,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1043,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1061,68 +1101,68 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
+      <c r="A12" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>111</v>
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>14</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>96</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>116</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>97</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1130,16 +1170,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>119</v>
+        <v>6</v>
+      </c>
+      <c r="D16" s="6">
+        <v>24</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1147,16 +1187,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>115</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="6">
+        <v>30</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1164,16 +1204,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>94</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="6">
+        <v>31</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1181,16 +1221,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>99</v>
+        <v>6</v>
+      </c>
+      <c r="D19" s="6">
+        <v>32</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1198,16 +1238,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>103</v>
+        <v>6</v>
+      </c>
+      <c r="D20" s="6">
+        <v>34</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1215,22 +1255,22 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>93</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="6">
+        <v>39</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1247,7 +1287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1264,7 +1304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1298,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1315,7 +1355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1332,7 +1372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1349,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1366,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1383,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1400,7 +1440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1417,7 +1457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
@@ -1434,7 +1474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -1451,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1468,7 +1508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1485,7 +1525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1502,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -1519,7 +1559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -1536,7 +1576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -1553,7 +1593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -1570,7 +1610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -1587,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -1604,7 +1644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1621,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -1638,7 +1678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -1655,7 +1695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -1672,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
@@ -1689,7 +1729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -1706,7 +1746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>60</v>
       </c>
@@ -1723,7 +1763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -1740,75 +1780,78 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>42</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="6">
+        <v>46</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="6">
+        <v>47</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52">
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="6">
         <v>62</v>
       </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53">
-        <v>61</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54">
-        <v>75</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55">
-        <v>42</v>
-      </c>
       <c r="E55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -1818,99 +1861,99 @@
       <c r="C56" t="s">
         <v>5</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="6">
         <v>58</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6">
+        <v>61</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6">
+        <v>63</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6">
+        <v>75</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6">
+        <v>74</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57">
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6">
         <v>80</v>
       </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58">
-        <v>74</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59">
-        <v>47</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60">
-        <v>63</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61">
-        <v>46</v>
-      </c>
       <c r="E61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -1927,7 +1970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -1944,7 +1987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -1961,7 +2004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -1978,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -1995,7 +2038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>77</v>
       </c>
@@ -2012,7 +2055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -2029,7 +2072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>79</v>
       </c>
@@ -2046,7 +2089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>80</v>
       </c>
@@ -2063,7 +2106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>81</v>
       </c>
@@ -2080,7 +2123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -2097,7 +2140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>83</v>
       </c>
@@ -2114,7 +2157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -2131,7 +2174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>85</v>
       </c>
@@ -2148,7 +2191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
@@ -2165,7 +2208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>87</v>
       </c>
@@ -2182,7 +2225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>88</v>
       </c>
@@ -2199,7 +2242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>89</v>
       </c>
@@ -2216,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>90</v>
       </c>
@@ -2233,7 +2276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>91</v>
       </c>
@@ -2250,7 +2293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>92</v>
       </c>
@@ -2267,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>93</v>
       </c>
@@ -2284,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>94</v>
       </c>
@@ -2301,7 +2344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>95</v>
       </c>
@@ -2318,7 +2361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>96</v>
       </c>
@@ -2335,7 +2378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>97</v>
       </c>
@@ -2352,7 +2395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>98</v>
       </c>
@@ -2369,7 +2412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>99</v>
       </c>
@@ -2386,7 +2429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>100</v>
       </c>
@@ -2403,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>101</v>
       </c>
@@ -2422,33 +2465,33 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="D92" s="6">
+        <v>93</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>103</v>
+      <c r="A93" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="D93" s="6">
+        <v>94</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -2456,33 +2499,33 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="D94" s="6">
+        <v>96</v>
       </c>
       <c r="E94">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>105</v>
+      <c r="A95" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D95">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -2490,33 +2533,33 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D96">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="E96">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>107</v>
+      <c r="A97" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -2524,16 +2567,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D98">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -2541,16 +2584,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D99">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2558,16 +2601,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D100">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2575,22 +2618,22 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D101">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="E101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>112</v>
       </c>
@@ -2607,7 +2650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>113</v>
       </c>
@@ -2624,7 +2667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>114</v>
       </c>
@@ -2641,7 +2684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>115</v>
       </c>
@@ -2658,7 +2701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>116</v>
       </c>
@@ -2675,7 +2718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>117</v>
       </c>
@@ -2692,7 +2735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>118</v>
       </c>
@@ -2709,7 +2752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>119</v>
       </c>
@@ -2726,7 +2769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>120</v>
       </c>
@@ -2743,7 +2786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>121</v>
       </c>
@@ -2760,7 +2803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>122</v>
       </c>
@@ -2777,7 +2820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>123</v>
       </c>
@@ -2794,7 +2837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>124</v>
       </c>
@@ -2811,7 +2854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>125</v>
       </c>
@@ -2828,7 +2871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>126</v>
       </c>
@@ -2845,7 +2888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>127</v>
       </c>
@@ -2862,7 +2905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>128</v>
       </c>
@@ -2879,7 +2922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>129</v>
       </c>
@@ -2896,7 +2939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>130</v>
       </c>
@@ -2913,7 +2956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>131</v>
       </c>
@@ -2930,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>132</v>
       </c>
@@ -2947,7 +2990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>133</v>
       </c>
@@ -2964,7 +3007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>134</v>
       </c>
@@ -2981,7 +3024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>135</v>
       </c>
@@ -2998,7 +3041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>136</v>
       </c>
@@ -3015,7 +3058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>137</v>
       </c>
@@ -3032,7 +3075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>138</v>
       </c>
@@ -3049,7 +3092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>139</v>
       </c>
@@ -3066,7 +3109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>140</v>
       </c>
@@ -3083,7 +3126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>141</v>
       </c>
@@ -3100,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>142</v>
       </c>
@@ -3117,8 +3160,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B133" t="s">
@@ -3134,77 +3177,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134">
+        <v>139</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" s="6">
+        <v>140</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136">
+        <v>148</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B134" t="s">
-        <v>2</v>
-      </c>
-      <c r="C134" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134">
+      <c r="B137" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="6">
         <v>149</v>
       </c>
-      <c r="E134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B135" t="s">
-        <v>2</v>
-      </c>
-      <c r="C135" t="s">
-        <v>7</v>
-      </c>
-      <c r="D135">
-        <v>157</v>
-      </c>
-      <c r="E135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B136" t="s">
-        <v>2</v>
-      </c>
-      <c r="C136" t="s">
-        <v>7</v>
-      </c>
-      <c r="D136">
-        <v>154</v>
-      </c>
-      <c r="E136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B137" t="s">
-        <v>2</v>
-      </c>
-      <c r="C137" t="s">
-        <v>7</v>
-      </c>
-      <c r="D137">
-        <v>139</v>
-      </c>
       <c r="E137">
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B138" t="s">
         <v>2</v>
@@ -3213,13 +3256,13 @@
         <v>7</v>
       </c>
       <c r="D138">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E138">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>149</v>
       </c>
@@ -3229,16 +3272,16 @@
       <c r="C139" t="s">
         <v>7</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="6">
         <v>152</v>
       </c>
       <c r="E139">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B140" t="s">
         <v>2</v>
@@ -3246,16 +3289,16 @@
       <c r="C140" t="s">
         <v>7</v>
       </c>
-      <c r="D140">
-        <v>140</v>
+      <c r="D140" s="6">
+        <v>154</v>
       </c>
       <c r="E140">
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B141" t="s">
         <v>2</v>
@@ -3264,13 +3307,14 @@
         <v>7</v>
       </c>
       <c r="D141">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141" s="7"/>
+    </row>
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>152</v>
       </c>
@@ -3287,7 +3331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>153</v>
       </c>
@@ -3304,7 +3348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>154</v>
       </c>
@@ -3321,7 +3365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>155</v>
       </c>
@@ -3338,7 +3382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>156</v>
       </c>
@@ -3355,7 +3399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>157</v>
       </c>
@@ -3372,7 +3416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>158</v>
       </c>
@@ -3389,7 +3433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>159</v>
       </c>
@@ -3406,7 +3450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>160</v>
       </c>
@@ -3423,7 +3467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>161</v>
       </c>
@@ -3440,7 +3484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>162</v>
       </c>
@@ -3457,7 +3501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>163</v>
       </c>
@@ -3474,7 +3518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>164</v>
       </c>
@@ -3491,7 +3535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>165</v>
       </c>
@@ -3508,7 +3552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>166</v>
       </c>
@@ -3525,7 +3569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>167</v>
       </c>
@@ -3542,7 +3586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>168</v>
       </c>
@@ -3559,7 +3603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>169</v>
       </c>
@@ -3576,7 +3620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>170</v>
       </c>
@@ -3593,7 +3637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>171</v>
       </c>
@@ -3611,6 +3655,21 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E161" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter val="**"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:E141">
+      <sortCondition ref="A1:A161"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>